<commit_message>
added functions to loop reports
</commit_message>
<xml_diff>
--- a/Template/input_template_lebanon_cs.xlsx
+++ b/Template/input_template_lebanon_cs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelfive/Desktop/R Directory/Git learning/MR-automation/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41CD77D-EBA8-5941-B855-7E35EA2E44E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF87BDD-0361-0F4B-BC23-1A241A534DBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{23A01AAA-5861-0842-AB9B-F1A19BD3FEAA}"/>
   </bookViews>
@@ -320,9 +320,6 @@
     <t>model_inv_age</t>
   </si>
   <si>
-    <t>model_lg_inv</t>
-  </si>
-  <si>
     <t>CS2_CFA4.out</t>
   </si>
   <si>
@@ -432,6 +429,9 @@
   </si>
   <si>
     <t>CS3_EFA.out</t>
+  </si>
+  <si>
+    <t>model_inv_lg</t>
   </si>
 </sst>
 </file>
@@ -814,7 +814,7 @@
         <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1106,7 +1106,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1120,7 +1120,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
@@ -1135,133 +1135,133 @@
         <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>94</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update template because box file path changed
</commit_message>
<xml_diff>
--- a/Template/input_template_lebanon_cs.xlsx
+++ b/Template/input_template_lebanon_cs.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelfive/Desktop/R Directory/Git learning/MR-automation/Template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF87BDD-0361-0F4B-BC23-1A241A534DBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A36C58E-C9F5-7A4F-9921-4C34C053CBE8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="460" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{23A01AAA-5861-0842-AB9B-F1A19BD3FEAA}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{23A01AAA-5861-0842-AB9B-F1A19BD3FEAA}"/>
   </bookViews>
   <sheets>
-    <sheet name="text" sheetId="1" r:id="rId1"/>
+    <sheet name="path" sheetId="1" r:id="rId1"/>
     <sheet name="subscale" sheetId="3" r:id="rId2"/>
     <sheet name="model" sheetId="4" r:id="rId3"/>
   </sheets>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="134">
   <si>
     <t>model_file_path</t>
   </si>
@@ -80,9 +80,6 @@
     <t>data_file_path</t>
   </si>
   <si>
-    <t>~/Box/3EA Analysis/3EA Lebanon_Analysis/Lebanon_Y1_FA/LBY1_PREIMPUTED_FULL_SPREAD_10-31-2019_mplus.dta</t>
-  </si>
-  <si>
     <t>HB1_AD_1</t>
   </si>
   <si>
@@ -416,9 +413,6 @@
     <t>CS123_CFA4_inv_scalar.out</t>
   </si>
   <si>
-    <t>~/Box/For Zezhen/MR automation/Test Data</t>
-  </si>
-  <si>
     <t>model_efa</t>
   </si>
   <si>
@@ -432,6 +426,18 @@
   </si>
   <si>
     <t>model_inv_lg</t>
+  </si>
+  <si>
+    <t>fs_data_file_path</t>
+  </si>
+  <si>
+    <t>/Users/michaelfive/Box/Box 3EA Team Folder/For Zezhen/MR automation/Test Data</t>
+  </si>
+  <si>
+    <t>/Users/michaelfive/Box/Box 3EA Team Folder/3EA Analysis/3EA Lebanon_Analysis/Lebanon_Y1_FA/LBY1_PREIMPUTED_FULL_SPREAD_10-31-2019_mplus.dta</t>
+  </si>
+  <si>
+    <t>/Users/michaelfive/Box/Box 3EA Team Folder/For Zezhen/MR automation/Test Data/CS123_fscores.csv</t>
   </si>
 </sst>
 </file>
@@ -783,19 +789,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C27BFF5F-7205-9748-9F48-9C16FDA3EB73}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="192" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="32.6640625" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -803,18 +810,24 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="C2" t="s">
-        <v>126</v>
+        <v>133</v>
+      </c>
+      <c r="D2" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -826,7 +839,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4276D3E0-CD11-5045-8B57-1997DA2EBF68}">
   <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView zoomScale="174" workbookViewId="0"/>
+    <sheetView zoomScale="174" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -838,34 +853,34 @@
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" t="s">
         <v>35</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>36</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>37</v>
       </c>
-      <c r="H1" t="s">
-        <v>38</v>
-      </c>
       <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -873,37 +888,37 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
         <v>39</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="H2" t="s">
-        <v>42</v>
-      </c>
       <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s">
         <v>67</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>68</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>69</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -911,37 +926,37 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F3" t="s">
         <v>43</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" t="s">
-        <v>46</v>
-      </c>
       <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
         <v>71</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>72</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>73</v>
-      </c>
-      <c r="L3" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -949,37 +964,37 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>49</v>
       </c>
-      <c r="H4" t="s">
-        <v>50</v>
-      </c>
       <c r="I4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J4" t="s">
         <v>75</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>76</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>77</v>
-      </c>
-      <c r="L4" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -987,37 +1002,37 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" t="s">
         <v>51</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>52</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>53</v>
       </c>
-      <c r="H5" t="s">
-        <v>54</v>
-      </c>
       <c r="I5" t="s">
+        <v>78</v>
+      </c>
+      <c r="J5" t="s">
         <v>79</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>80</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>81</v>
-      </c>
-      <c r="L5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1025,37 +1040,37 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
         <v>55</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>56</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>57</v>
       </c>
-      <c r="H6" t="s">
-        <v>58</v>
-      </c>
       <c r="I6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J6" t="s">
         <v>83</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>84</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>85</v>
-      </c>
-      <c r="L6" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -1063,37 +1078,37 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>60</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>61</v>
       </c>
-      <c r="H7" t="s">
-        <v>62</v>
-      </c>
       <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" t="s">
         <v>87</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>88</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>89</v>
-      </c>
-      <c r="L7" t="s">
-        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1105,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{601705C5-50A2-7A46-BFF2-1E1E17DB5A98}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="209" workbookViewId="0">
+    <sheetView zoomScale="209" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
@@ -1120,148 +1135,148 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>
       </c>
       <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" t="s">
-        <v>93</v>
-      </c>
       <c r="F1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E6" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E10" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>